<commit_message>
Version 0.37: SECURITY UPDATE
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,51 +427,6 @@
           <t>mac-адрес</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>03.11.23</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Миша</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>50:ff:20:a0:e3:c4</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>52:ff:20:a0:e3:c3</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>04:7c:16:3e:cc:79</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>9.68</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>